<commit_message>
Update Power BI Report Process
</commit_message>
<xml_diff>
--- a/Power BI Report Process/Report.3.0.17/Data/Config.xlsx
+++ b/Power BI Report Process/Report.3.0.17/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\986011\Desktop\UiPath\Report\Report\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\561625\Documents\GitHub\UiPath-Work\Power BI Report Process\Report.3.0.17\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D551D0AC-3316-4D1D-8DD5-F6E83A38A470}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593A7187-C2A1-4CE6-BCB2-A6959D2845F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26700" yWindow="-165" windowWidth="13725" windowHeight="9435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -534,15 +534,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.81640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -601,7 +601,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.5">
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1630,12 +1630,12 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.36328125" customWidth="1"/>
-    <col min="4" max="26" width="8.81640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1672,7 +1672,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2736,18 +2736,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="35.7265625" customWidth="1"/>
-    <col min="2" max="2" width="36.36328125" customWidth="1"/>
-    <col min="3" max="3" width="77.08984375" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="77.140625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2827,8 +2827,16 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3816,7 +3824,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>